<commit_message>
unexpected behaviour - add new column with value c instated of adding/updating cell - A3 with value c
</commit_message>
<xml_diff>
--- a/example/poly1.xlsx
+++ b/example/poly1.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{E5D66FDA-5372-4962-86E8-3BA28A34DBE9}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{6E5F0601-4379-4C17-AC62-823987DEC16B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2400" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="3000" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -346,7 +346,7 @@
   <dimension ref="A1:B70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -358,21 +358,6 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>c</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>c</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>c</t>
-        </is>
-      </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">

</xml_diff>